<commit_message>
Update herolist to latest version
</commit_message>
<xml_diff>
--- a/excels/英雄列表.xlsx
+++ b/excels/英雄列表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\x-template\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\x-template\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC75D775-534B-40A9-8C91-B72DCAD29009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2FD333-7DDC-40BB-95F8-3722FD9EC8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="323" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>npc_dota_hero_earthshaker</t>
   </si>
@@ -409,6 +409,27 @@
   <si>
     <t>这种只有两列的表，会直接转成 "npc_dota_hero_ancient_apparition" "1"的形式</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>npc_dota_hero_hoodwink</t>
+  </si>
+  <si>
+    <t>npc_dota_hero_dawnbreaker</t>
+  </si>
+  <si>
+    <t>npc_dota_hero_marci</t>
+  </si>
+  <si>
+    <t>npc_dota_hero_primal_beast</t>
+  </si>
+  <si>
+    <t>npc_dota_hero_muerta</t>
+  </si>
+  <si>
+    <t>npc_dota_hero_ringmaster</t>
+  </si>
+  <si>
+    <t>npc_dota_hero_kez</t>
   </si>
 </sst>
 </file>
@@ -779,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29C7AE1-1213-469D-856F-83D4B90AB9D9}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1762,6 +1783,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>